<commit_message>
GOOD DATA FOR 8 GANTT CHARTS
</commit_message>
<xml_diff>
--- a/for Hector/Tom/mrn1Left.xlsx
+++ b/for Hector/Tom/mrn1Left.xlsx
@@ -479,10 +479,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -1098,7 +1109,7 @@
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1124,10 +1135,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1136,27 +1147,27 @@
         <v>12</v>
       </c>
       <c r="E23" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
         <v>13</v>
       </c>
       <c r="H23" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1168,16 +1179,16 @@
         <v>2012</v>
       </c>
       <c r="F24" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <v>13</v>
       </c>
       <c r="H24" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:9">

</xml_diff>